<commit_message>
Salario promedio por especialización
</commit_message>
<xml_diff>
--- a/dataset_empleados_limpio.xlsx
+++ b/dataset_empleados_limpio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Isaías\Desktop\3er año - 2023\Probabilidad y Estadística\IntegradorPE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1AE9D2-7529-4626-A650-ADE40AB437B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C5A988-4373-4274-95FD-0F0AB05F88D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>